<commit_message>
Domino Single Ethernet tile Revision B
</commit_message>
<xml_diff>
--- a/Domino Single Ethernet/BOM/Domino Single Ethernet BOM.xlsx
+++ b/Domino Single Ethernet/BOM/Domino Single Ethernet BOM.xlsx
@@ -11,32 +11,33 @@
     <sheet name="Domino Single Ethernet Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Item</t>
   </si>
@@ -65,39 +66,39 @@
     <t>Remarks</t>
   </si>
   <si>
+    <t>2n2</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>C1210_2n2_X7R_10%_CER_2kV</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>CAP CER 2200PF 1KV 10% X7R 1210</t>
+  </si>
+  <si>
     <t>100n</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>C0402_100n_X7R_10%_CER_50V</t>
   </si>
   <si>
     <t>C0402</t>
   </si>
   <si>
-    <t>C1, C2, C4</t>
+    <t>C3, C4, C5</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
   </si>
   <si>
-    <t>2n2</t>
-  </si>
-  <si>
-    <t>C1210_2n2_X7R_10%_CER_2kV</t>
-  </si>
-  <si>
-    <t>C1206</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>CAP CER 2200PF 1KV 10% X7R 1210</t>
-  </si>
-  <si>
     <t>BLUE</t>
   </si>
   <si>
@@ -167,30 +168,30 @@
     <t>LED YELLOW CLEAR 0603 SMD</t>
   </si>
   <si>
+    <t>11A009-1702-00</t>
+  </si>
+  <si>
+    <t>MENTECH</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CONN MAGJACK 1PORT 100 BASE-T</t>
+  </si>
+  <si>
     <t>MH18-1</t>
   </si>
   <si>
     <t>MH18-1-0.1</t>
   </si>
   <si>
-    <t>J1, J2</t>
+    <t>J2, J3</t>
   </si>
   <si>
     <t>CONN HEADER VERT .100 1ROW 18POS 8.08 HEAD 3.05 TAIL 15AU</t>
   </si>
   <si>
-    <t>B50(27-51)FP4-151-A613-B12</t>
-  </si>
-  <si>
-    <t>BROADTOP ELECTRONIC</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>CONN MAGJACK 1PORT 100 BASE-T</t>
-  </si>
-  <si>
     <t>49R9</t>
   </si>
   <si>
@@ -206,28 +207,16 @@
     <t>RES 49.9 OHM 1/16W 1% 0402 SMD</t>
   </si>
   <si>
-    <t>150R</t>
-  </si>
-  <si>
-    <t>R0603_150R_5%_125mW</t>
+    <t>330R</t>
+  </si>
+  <si>
+    <t>R0603_330R_5%_125mW</t>
   </si>
   <si>
     <t>R0603</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>RES 150 OHM 1/8W 5% 0603 SMD</t>
-  </si>
-  <si>
-    <t>330R</t>
-  </si>
-  <si>
-    <t>R0603_330R_5%_125mW</t>
-  </si>
-  <si>
-    <t>R5, R13, R14</t>
+    <t>R11, R12, R13</t>
   </si>
   <si>
     <t>RES 330 OHM 1/8W 5% 0603 SMD</t>
@@ -239,7 +228,7 @@
     <t>R0603_270R_5%_125mW</t>
   </si>
   <si>
-    <t>R6, R7, R8, R9, R10, R11</t>
+    <t>R5, R6, R7, R8, R9, R10</t>
   </si>
   <si>
     <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
@@ -353,22 +342,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.92941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.643137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.9607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.0078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.95294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.1607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.5450980392157"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -405,7 +394,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -431,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>15</v>
@@ -613,19 +602,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>45</v>
@@ -639,19 +628,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>49</v>
@@ -691,7 +680,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>56</v>
@@ -717,7 +706,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>61</v>
@@ -736,32 +725,6 @@
       </c>
       <c r="H14" s="0" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino Single Ethernet Rev. C: changed Logos
</commit_message>
<xml_diff>
--- a/Domino Single Ethernet/BOM/Domino Single Ethernet BOM.xlsx
+++ b/Domino Single Ethernet/BOM/Domino Single Ethernet BOM.xlsx
@@ -8,29 +8,30 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Single Ethernet Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Single Ethernet Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -349,15 +350,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.1607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.5450980392157"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.043137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.043137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3686274509804"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Domnio Single Ethernet Rev. D: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino Single Ethernet/BOM/Domino Single Ethernet BOM.xlsx
+++ b/Domino Single Ethernet/BOM/Domino Single Ethernet BOM.xlsx
@@ -8,30 +8,31 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Single Ethernet Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Single Ethernet Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single Ethernet Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -350,14 +351,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.043137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.043137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3686274509804"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.1764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.5764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.1803921568628"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3882352941176"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>